<commit_message>
new bug created, new testcase created
Signed-off-by: muellers <stefan.mueller@vol.at>
</commit_message>
<xml_diff>
--- a/testing/Bugs.xlsx
+++ b/testing/Bugs.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Kunde ohne Name und Adresse kann erstellt werden (die zwei Felder sollten zumindes Pflichtfelder sein)</t>
+  </si>
+  <si>
+    <t>Löschen eines Kunden mit Reservierung führt zu Exception =&gt; das sollte abgefangen werden u. eine Fehlermeldung ausgegeben werden: "Kunde kann nicht glöscht werden...."</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <dimension ref="A1:W174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -680,12 +683,25 @@
       </c>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
+    <row r="5" spans="1:23" ht="90">
+      <c r="A5" s="10">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>

</xml_diff>

<commit_message>
Update bugs; preparations for issue #6
The preparations in ObjectList depend on new DAO
methods that are not yet implemented.

DAO methods missing: See Issue #14 and Issue #15.
</commit_message>
<xml_diff>
--- a/testing/Bugs.xlsx
+++ b/testing/Bugs.xlsx
@@ -108,7 +108,7 @@
     <t>Martin</t>
   </si>
   <si>
-    <t>Löschen eines Kunden mit Reservierung führt zu Exception =&gt; das sollte abgefangen werden u. eine Fehlermeldung ausgegeben werden: "Kunde kann nicht glöscht werden...."</t>
+    <t>Löschen eines Kunden mit Reservierung führt zu Exception =&gt; das sollte abgefangen werden u. eine Fehlermeldung ausgegeben werden: "Kunde kann nicht glöscht werden...."; Re-assigned zu Martin: DAO-Methode (siehe Issue 14)</t>
   </si>
   <si>
     <t>Retest</t>
@@ -117,7 +117,7 @@
     <t>CRUD Zimmer</t>
   </si>
   <si>
-    <t>Löschen eines Zimmer mit Reservierung führt zu Exception =&gt; das sollte abgefangen werden u. eine Fehlermeldung ausgegeben werden: "Zimmer kann nicht gelöscht werden...."</t>
+    <t>Löschen eines Zimmer mit Reservierung führt zu Exception =&gt; das sollte abgefangen werden u. eine Fehlermeldung ausgegeben werden: "Zimmer kann nicht gelöscht werden...."; Re-assigned zu Martin: DAO-Methode (siehe Issue 15)</t>
   </si>
   <si>
     <t>Retest NOK</t>
@@ -201,6 +201,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="12"/>
@@ -216,7 +217,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00C6D9F1"/>
-        <bgColor rgb="0099CCFF"/>
+        <bgColor rgb="00C0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -336,7 +337,7 @@
       <rgbColor rgb="00808000"/>
       <rgbColor rgb="00800080"/>
       <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C3D69B"/>
+      <rgbColor rgb="00C0C0C0"/>
       <rgbColor rgb="00808080"/>
       <rgbColor rgb="009999FF"/>
       <rgbColor rgb="00993366"/>
@@ -361,7 +362,7 @@
       <rgbColor rgb="0099CCFF"/>
       <rgbColor rgb="00FF99CC"/>
       <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00E6B9B8"/>
+      <rgbColor rgb="00FFCC99"/>
       <rgbColor rgb="003366FF"/>
       <rgbColor rgb="0033CCCC"/>
       <rgbColor rgb="0099CC00"/>
@@ -383,14 +384,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
-</file>
-
-<file path=xl/drawings/vmlDrawing1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<xml xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:x="urn:schemas-microsoft-com:office:excel"><v:shapetype id="shapetype_75" coordsize="21600,21600" o:spt="75" adj="2700" path="m,l21600,l21600,21600l,21600xm@0@0l@0@2l@1@2l@1@0xe"><v:stroke joinstyle="miter"/><v:formulas><v:f eqn="val #0"/><v:f eqn="sum width 0 @0"/><v:f eqn="sum height 0 @0"/></v:formulas><v:path gradientshapeok="t" o:connecttype="rect" textboxrect="@0,@0,@1,@2"/><v:handles><v:h position="@0,0"/></v:handles></v:shapetype><v:shape id="shape_0" style="position:absolute;margin-left:658.8pt;margin-top:21.1pt;width:142.75pt;height:51.25pt;visibility:hidden" type="shapetype_75"><w10:wrap w10:type="none"/><v:fill color="#ffffe1" color2="#00001e" detectmouseclick="t" type="solid"/><v:stroke color="black" joinstyle="miter" startarrow="block" startarrowlength="medium" startarrowwidth="medium"/><x:ClientData ObjectType="Note"><x:MoveWithCells/><x:SizeWithCells/><x:Anchor>4, 91, 1, 10, 22, 22, 3, 35</x:Anchor><x:AutoFill>False</x:AutoFill><x:Row>2</x:Row><x:Column>4</x:Column></x:ClientData></v:shape><v:shapetype id="shapetype_75" coordsize="21600,21600" o:spt="75" adj="2700" path="m,l21600,l21600,21600l,21600xm@0@0l@0@2l@1@2l@1@0xe"><v:stroke joinstyle="miter"/><v:formulas><v:f eqn="val #0"/><v:f eqn="sum width 0 @0"/><v:f eqn="sum height 0 @0"/></v:formulas><v:path gradientshapeok="t" o:connecttype="rect" textboxrect="@0,@0,@1,@2"/><v:handles><v:h position="@0,0"/></v:handles></v:shapetype><v:shape id="shape_0" style="position:absolute;margin-left:676.65pt;margin-top:21.1pt;width:142.75pt;height:51.25pt;visibility:hidden" type="shapetype_75"><w10:wrap w10:type="none"/><v:fill color="#ffffe1" color2="#00001e" detectmouseclick="t" type="solid"/><v:stroke color="black" joinstyle="miter" startarrow="block" startarrowlength="medium" startarrowwidth="medium"/><x:ClientData ObjectType="Note"><x:MoveWithCells/><x:SizeWithCells/><x:Anchor>4, 114, 1, 10, 22, 46, 3, 35</x:Anchor><x:AutoFill>False</x:AutoFill><x:Row>2</x:Row><x:Column>5</x:Column></x:ClientData></v:shape></xml>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -399,18 +392,19 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
+      <selection activeCell="E7" activeCellId="0" pane="topLeft" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5411764705882"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5411764705882"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.121568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="33.3921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.8862745098039"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.2078431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.2666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="33.5294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.9843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.24313725490196"/>
     <col collapsed="false" hidden="true" max="22" min="7" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="257" min="23" style="0" width="8.6078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="23" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -434,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="18.4" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -460,7 +454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="38.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="42.1" outlineLevel="0" r="4">
       <c r="A4" s="10" t="n">
         <v>1</v>
       </c>
@@ -477,7 +471,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -501,7 +495,7 @@
       </c>
       <c r="W4" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="65.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="95.65" outlineLevel="0" r="5">
       <c r="A5" s="10" t="n">
         <v>2</v>
       </c>
@@ -515,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>1</v>
@@ -542,7 +536,7 @@
       </c>
       <c r="W5" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.2" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="95.65" outlineLevel="0" r="6">
       <c r="A6" s="10" t="n">
         <v>3</v>
       </c>
@@ -556,7 +550,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>1</v>
@@ -583,7 +577,7 @@
       </c>
       <c r="W6" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="27.85" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="7">
       <c r="A7" s="10" t="n">
         <v>4</v>
       </c>
@@ -624,7 +618,7 @@
       </c>
       <c r="W7" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.3" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="8">
       <c r="A8" s="10" t="n">
         <v>5</v>
       </c>
@@ -665,7 +659,7 @@
       </c>
       <c r="W8" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.3" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="9">
       <c r="A9" s="10" t="n">
         <v>6</v>
       </c>
@@ -702,7 +696,7 @@
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.3" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="10">
       <c r="A10" s="10" t="n">
         <v>7</v>
       </c>
@@ -739,7 +733,7 @@
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.3" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="11">
       <c r="A11" s="10" t="n">
         <v>8</v>
       </c>
@@ -776,7 +770,7 @@
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.3" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="12">
       <c r="A12" s="10" t="n">
         <v>9</v>
       </c>
@@ -814,8 +808,6 @@
       <c r="W12" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:V3"/>
-  <conditionalFormatting sqref="F4:F46"/>
   <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F7" type="list">
       <formula1>$T$2:$T$4</formula1>
@@ -837,8 +829,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -854,7 +845,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.6078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -879,7 +871,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.6078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>